<commit_message>
refactoring of toolbox components
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/vsme/vsme.xlsx
+++ b/dataland-framework-toolbox/inputs/vsme/vsme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\sme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\vsme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8502B2A1-3AF3-4DDA-BF34-B8D9BE05B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C50BBC-EA8B-41D3-8E42-0C76F16C0EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-11000" windowWidth="25820" windowHeight="14020" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -930,15 +930,9 @@
     <t>Cubic Meters</t>
   </si>
   <si>
-    <t>Sme Subsidiary</t>
-  </si>
-  <si>
     <t>Total nature-oriented area off-site previous year</t>
   </si>
   <si>
-    <t>Sme Pollution Emission</t>
-  </si>
-  <si>
     <t>Pollution Emission</t>
   </si>
   <si>
@@ -948,9 +942,6 @@
     <t>HeadCount</t>
   </si>
   <si>
-    <t>Sme Site And Area</t>
-  </si>
-  <si>
     <t>Sites and Areas</t>
   </si>
   <si>
@@ -1060,6 +1051,15 @@
   </si>
   <si>
     <t>Please provide the entry level wage you pay.</t>
+  </si>
+  <si>
+    <t>Vsme Subsidiary</t>
+  </si>
+  <si>
+    <t>Vsme Pollution Emission</t>
+  </si>
+  <si>
+    <t>Vsme Site And Area</t>
   </si>
 </sst>
 </file>
@@ -1653,9 +1653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE53926-978F-4910-9169-F720F1E0A6DD}">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="27" t="s">
-        <v>288</v>
+        <v>329</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1785,23 +1785,23 @@
         <v>274</v>
       </c>
       <c r="D4" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>299</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>300</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>302</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="27" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -2089,14 +2089,14 @@
         <v>277</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="19" t="s">
-        <v>290</v>
+        <v>330</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2117,14 +2117,14 @@
         <v>278</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="31" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2313,7 +2313,7 @@
         <v>278</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>81</v>
@@ -2879,12 +2879,12 @@
         <v>283</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -2935,7 +2935,7 @@
         <v>282</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>166</v>
@@ -2953,7 +2953,7 @@
         <v>112</v>
       </c>
       <c r="L44" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
@@ -2969,7 +2969,7 @@
         <v>282</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>166</v>
@@ -2987,7 +2987,7 @@
         <v>112</v>
       </c>
       <c r="L45" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
@@ -3003,7 +3003,7 @@
         <v>282</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>173</v>
@@ -3021,7 +3021,7 @@
         <v>112</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
@@ -3037,7 +3037,7 @@
         <v>282</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>173</v>
@@ -3055,7 +3055,7 @@
         <v>112</v>
       </c>
       <c r="L47" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
@@ -3071,7 +3071,7 @@
         <v>282</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -3087,7 +3087,7 @@
         <v>112</v>
       </c>
       <c r="L48" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
@@ -3103,7 +3103,7 @@
         <v>282</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
@@ -3119,7 +3119,7 @@
         <v>112</v>
       </c>
       <c r="L49" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
@@ -3135,7 +3135,7 @@
         <v>282</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>178</v>
@@ -3153,7 +3153,7 @@
         <v>112</v>
       </c>
       <c r="L50" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
@@ -3169,7 +3169,7 @@
         <v>282</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>178</v>
@@ -3187,7 +3187,7 @@
         <v>112</v>
       </c>
       <c r="L51" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
@@ -3203,7 +3203,7 @@
         <v>282</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -3219,7 +3219,7 @@
         <v>112</v>
       </c>
       <c r="L52" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
@@ -3235,7 +3235,7 @@
         <v>282</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -3251,7 +3251,7 @@
         <v>112</v>
       </c>
       <c r="L53" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
@@ -3267,7 +3267,7 @@
         <v>282</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3283,7 +3283,7 @@
         <v>112</v>
       </c>
       <c r="L54" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
@@ -3299,7 +3299,7 @@
         <v>282</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -3315,7 +3315,7 @@
         <v>112</v>
       </c>
       <c r="L55" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
@@ -3331,7 +3331,7 @@
         <v>282</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
@@ -3347,7 +3347,7 @@
         <v>112</v>
       </c>
       <c r="L56" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
@@ -3363,7 +3363,7 @@
         <v>282</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
@@ -3379,7 +3379,7 @@
         <v>112</v>
       </c>
       <c r="L57" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="2"/>
@@ -3395,14 +3395,14 @@
         <v>282</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>187</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -3453,7 +3453,7 @@
         <v>281</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>198</v>
@@ -3509,7 +3509,7 @@
         <v>281</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>204</v>
@@ -3527,7 +3527,7 @@
         <v>112</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
@@ -3543,7 +3543,7 @@
         <v>281</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>204</v>
@@ -3561,7 +3561,7 @@
         <v>112</v>
       </c>
       <c r="L63" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
@@ -3577,7 +3577,7 @@
         <v>281</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>207</v>
@@ -3595,7 +3595,7 @@
         <v>112</v>
       </c>
       <c r="L64" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
@@ -3611,7 +3611,7 @@
         <v>281</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>207</v>
@@ -3629,7 +3629,7 @@
         <v>112</v>
       </c>
       <c r="L65" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
@@ -3645,7 +3645,7 @@
         <v>281</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
@@ -3661,7 +3661,7 @@
         <v>112</v>
       </c>
       <c r="L66" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
@@ -3677,7 +3677,7 @@
         <v>281</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
@@ -3693,7 +3693,7 @@
         <v>112</v>
       </c>
       <c r="L67" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
@@ -3709,7 +3709,7 @@
         <v>280</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>212</v>
@@ -3727,7 +3727,7 @@
         <v>112</v>
       </c>
       <c r="L68" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
@@ -3743,7 +3743,7 @@
         <v>280</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>212</v>
@@ -3761,7 +3761,7 @@
         <v>112</v>
       </c>
       <c r="L69" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M69" s="9"/>
       <c r="N69" s="2"/>
@@ -3777,7 +3777,7 @@
         <v>280</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>215</v>
@@ -3805,7 +3805,7 @@
         <v>280</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>216</v>
@@ -3836,7 +3836,7 @@
         <v>217</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
@@ -3866,7 +3866,7 @@
         <v>219</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
@@ -4271,7 +4271,7 @@
         <v>112</v>
       </c>
       <c r="L85" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
@@ -4305,7 +4305,7 @@
         <v>112</v>
       </c>
       <c r="L86" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M86" s="9"/>
       <c r="N86" s="2"/>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="9" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>

</xml_diff>

<commit_message>
updates datamodel after sanitycheck
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/vsme/vsme.xlsx
+++ b/dataland-framework-toolbox/inputs/vsme/vsme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\vsme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCD1E6F-CD0B-4EB6-AC02-E0C9B3420C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ECEEF6-D5A3-4BF1-9030-CDE483C6B7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="365">
   <si>
     <t>1</t>
   </si>
@@ -85,10 +85,6 @@
     <t>Energy Fossil Fuels</t>
   </si>
   <si>
-    <t xml:space="preserve">Please disclose your total energy consumption in MWh (in the reporting period) for
-- fossil fuels </t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -96,9 +92,6 @@
   </si>
   <si>
     <t>4</t>
-  </si>
-  <si>
-    <t>- electricity as reflected in utility billings. If available distinguish between renewable and non_x0002_renewable sources.</t>
   </si>
   <si>
     <t>5</t>
@@ -828,39 +821,24 @@
     <t>Electricity Renewable</t>
   </si>
   <si>
-    <t>Total Aealed Area Previous Year</t>
-  </si>
-  <si>
     <t>Total Sealed Area Reporting Year</t>
   </si>
   <si>
-    <t>Percentual Change Sealed Area</t>
-  </si>
-  <si>
     <t>Total Nature-Oriented Area On-Site Reporting Year</t>
   </si>
   <si>
-    <t>Percentual Change Nature-Oriented On-Site</t>
-  </si>
-  <si>
     <t>Total Nature-Oriented Area Off-Site Previous Year</t>
   </si>
   <si>
     <t>Total Nature-Oriented Area Off-Site Reporting Year</t>
   </si>
   <si>
-    <t>Percentual Change Nature-Oriented Off-Site</t>
-  </si>
-  <si>
     <t>Total Use Of Land Previous Year</t>
   </si>
   <si>
     <t>Total Use Of Land Reporting Year</t>
   </si>
   <si>
-    <t>Percentual Change Land Use</t>
-  </si>
-  <si>
     <t>Water Withdrawal All Sites</t>
   </si>
   <si>
@@ -1156,6 +1134,30 @@
   </si>
   <si>
     <t>Number Bargaining Agreements  In FTE</t>
+  </si>
+  <si>
+    <t>Please disclose your total energy consumption in MWh (in the reporting period) for fossil fuels.</t>
+  </si>
+  <si>
+    <t>Please disclose your total energy consumption in MWh (in the reporting period) for electricity as reflected in utility billings. If available distinguish between renewable and non_x0002_renewable sources.</t>
+  </si>
+  <si>
+    <t>Relative Change Sealed Area</t>
+  </si>
+  <si>
+    <t>Relative Change Nature-Oriented On-Site</t>
+  </si>
+  <si>
+    <t>Relative Change Nature-Oriented Off-Site</t>
+  </si>
+  <si>
+    <t>Total Sealed Area Previous Year</t>
+  </si>
+  <si>
+    <t>Relative Change Land Use</t>
+  </si>
+  <si>
+    <t>Please disclose the waste classification for every type of waste.</t>
   </si>
 </sst>
 </file>
@@ -1765,8 +1767,8 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1787,43 +1789,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>
@@ -1832,10 +1834,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1862,20 +1864,20 @@
         <v>11</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1890,50 +1892,50 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D4" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="G4" s="32" t="s">
         <v>240</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>242</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>219</v>
-      </c>
       <c r="D5" s="27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1943,29 +1945,29 @@
       <c r="M5" s="3"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
+      <c r="E6" s="28" t="s">
+        <v>357</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="12"/>
@@ -1973,32 +1975,32 @@
       <c r="M6" s="3"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>18</v>
+        <v>358</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="11"/>
@@ -2007,27 +2009,27 @@
     </row>
     <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="12"/>
@@ -2037,27 +2039,27 @@
     </row>
     <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="12"/>
@@ -2067,30 +2069,30 @@
     </row>
     <row r="10" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
@@ -2099,30 +2101,30 @@
     </row>
     <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
@@ -2131,30 +2133,30 @@
     </row>
     <row r="12" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
@@ -2163,30 +2165,30 @@
     </row>
     <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="11"/>
@@ -2195,23 +2197,23 @@
     </row>
     <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2223,23 +2225,23 @@
     </row>
     <row r="15" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2251,27 +2253,27 @@
     </row>
     <row r="16" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>254</v>
+        <v>362</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="28" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -2281,27 +2283,27 @@
     </row>
     <row r="17" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -2311,23 +2313,23 @@
     </row>
     <row r="18" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>256</v>
+        <v>359</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2339,27 +2341,27 @@
     </row>
     <row r="19" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -2369,27 +2371,27 @@
     </row>
     <row r="20" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -2399,23 +2401,23 @@
     </row>
     <row r="21" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>258</v>
+        <v>360</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2427,27 +2429,27 @@
     </row>
     <row r="22" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -2457,27 +2459,27 @@
     </row>
     <row r="23" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -2487,23 +2489,23 @@
     </row>
     <row r="24" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>261</v>
+        <v>361</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -2515,27 +2517,27 @@
     </row>
     <row r="25" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -2545,27 +2547,27 @@
     </row>
     <row r="26" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -2575,23 +2577,23 @@
     </row>
     <row r="27" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A27" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>264</v>
+        <v>363</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -2603,30 +2605,30 @@
     </row>
     <row r="28" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -2635,27 +2637,27 @@
     </row>
     <row r="29" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2665,27 +2667,27 @@
     </row>
     <row r="30" spans="1:14" ht="88" x14ac:dyDescent="0.35">
       <c r="A30" s="35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2695,27 +2697,27 @@
     </row>
     <row r="31" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2725,27 +2727,27 @@
     </row>
     <row r="32" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2755,27 +2757,27 @@
     </row>
     <row r="33" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2785,27 +2787,27 @@
     </row>
     <row r="34" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2815,27 +2817,27 @@
     </row>
     <row r="35" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -2845,27 +2847,27 @@
     </row>
     <row r="36" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A36" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -2875,27 +2877,27 @@
     </row>
     <row r="37" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -2905,23 +2907,23 @@
     </row>
     <row r="38" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -2933,27 +2935,27 @@
     </row>
     <row r="39" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -2963,23 +2965,23 @@
     </row>
     <row r="40" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -2991,26 +2993,26 @@
     </row>
     <row r="41" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="2"/>
@@ -3021,21 +3023,23 @@
     </row>
     <row r="42" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="E42" s="9"/>
+        <v>235</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>364</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -3047,26 +3051,26 @@
     </row>
     <row r="43" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -3077,499 +3081,499 @@
     </row>
     <row r="44" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L44" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L45" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L47" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" s="35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L48" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L49" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L50" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L51" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L52" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
     </row>
     <row r="53" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L53" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L54" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L55" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
     </row>
     <row r="56" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" s="9"/>
       <c r="I56" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L56" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
     </row>
     <row r="57" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H57" s="9"/>
       <c r="I57" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L57" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -3581,27 +3585,27 @@
     </row>
     <row r="59" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -3611,23 +3615,23 @@
     </row>
     <row r="60" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
@@ -3639,23 +3643,23 @@
     </row>
     <row r="61" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
@@ -3667,295 +3671,295 @@
     </row>
     <row r="62" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
     </row>
     <row r="63" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L63" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L64" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
     </row>
     <row r="65" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L65" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
     </row>
     <row r="66" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H66" s="9"/>
       <c r="I66" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L66" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
     </row>
     <row r="67" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H67" s="9"/>
       <c r="I67" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L67" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
     </row>
     <row r="68" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L68" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L69" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M69" s="9"/>
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -3967,19 +3971,19 @@
     </row>
     <row r="71" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
@@ -3995,27 +3999,27 @@
     </row>
     <row r="72" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -4025,27 +4029,27 @@
     </row>
     <row r="73" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -4055,23 +4059,23 @@
     </row>
     <row r="74" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -4083,26 +4087,26 @@
     </row>
     <row r="75" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
@@ -4110,302 +4114,302 @@
         <v>43</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M75" s="9"/>
       <c r="N75" s="2"/>
     </row>
     <row r="76" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="8">
         <v>43</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M76" s="9"/>
       <c r="N76" s="2"/>
     </row>
     <row r="77" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F77" s="9"/>
       <c r="G77" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="8">
         <v>43</v>
       </c>
       <c r="L77" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M77" s="9"/>
       <c r="N77" s="2"/>
     </row>
     <row r="78" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A78" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H78" s="9"/>
       <c r="I78" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="8">
         <v>43</v>
       </c>
       <c r="L78" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M78" s="9"/>
       <c r="N78" s="2"/>
     </row>
     <row r="79" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A79" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="8">
         <v>43</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M79" s="9"/>
       <c r="N79" s="2"/>
     </row>
     <row r="80" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A80" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H80" s="9"/>
       <c r="I80" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="8">
         <v>43</v>
       </c>
       <c r="L80" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M80" s="9"/>
       <c r="N80" s="2"/>
     </row>
     <row r="81" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H81" s="9"/>
       <c r="I81" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="8">
         <v>43</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M81" s="9"/>
       <c r="N81" s="2"/>
     </row>
     <row r="82" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H82" s="9"/>
       <c r="I82" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="8">
         <v>43</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M82" s="9"/>
       <c r="N82" s="2"/>
     </row>
     <row r="83" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F83" s="9"/>
       <c r="G83" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J83" s="9"/>
       <c r="K83" s="8">
         <v>43</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M83" s="9"/>
       <c r="N83" s="2"/>
     </row>
     <row r="84" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F84" s="9"/>
       <c r="G84" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
@@ -4414,98 +4418,98 @@
         <v>43</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
     </row>
     <row r="85" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F85" s="9"/>
       <c r="G85" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="J85" s="9"/>
       <c r="K85" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L85" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
     </row>
     <row r="86" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A86" s="35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F86" s="9"/>
       <c r="G86" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H86" s="9"/>
       <c r="I86" s="28" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="J86" s="9"/>
       <c r="K86" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L86" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M86" s="9"/>
       <c r="N86" s="2"/>
     </row>
     <row r="87" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H87" s="9"/>
       <c r="I87" s="9"/>
@@ -4517,27 +4521,27 @@
     </row>
     <row r="88" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A88" s="35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="F88" s="9"/>
       <c r="G88" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H88" s="9"/>
       <c r="I88" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
@@ -4547,27 +4551,27 @@
     </row>
     <row r="89" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A89" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="E89" s="28" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F89" s="9"/>
       <c r="G89" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H89" s="9"/>
       <c r="I89" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -4577,27 +4581,27 @@
     </row>
     <row r="90" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A90" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E90" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F90" s="9"/>
       <c r="G90" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H90" s="9"/>
       <c r="I90" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
@@ -4607,27 +4611,27 @@
     </row>
     <row r="91" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A91" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E91" s="28" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F91" s="9"/>
       <c r="G91" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H91" s="9"/>
       <c r="I91" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J91" s="2"/>
       <c r="K91" s="9"/>
@@ -4637,23 +4641,23 @@
     </row>
     <row r="92" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A92" s="35" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
@@ -4665,23 +4669,23 @@
     </row>
     <row r="93" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A93" s="34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H93" s="9"/>
       <c r="I93" s="9"/>
@@ -4693,25 +4697,25 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C94" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D94" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E94" s="37" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="G94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4738,70 +4742,70 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -4810,16 +4814,16 @@
     </row>
     <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -4836,192 +4840,192 @@
     </row>
     <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="2"/>
@@ -5052,58 +5056,58 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
@@ -5120,16 +5124,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
@@ -5146,21 +5150,21 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -5172,21 +5176,21 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -5198,21 +5202,21 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -5224,25 +5228,25 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -5252,16 +5256,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -5278,16 +5282,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -5304,21 +5308,21 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -5330,21 +5334,21 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -5356,24 +5360,24 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -5408,63 +5412,63 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -5476,64 +5480,64 @@
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="2"/>
@@ -5562,63 +5566,63 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
       <c r="G2" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -5630,25 +5634,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
       <c r="G3" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="12"/>
@@ -5658,24 +5662,24 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
       <c r="G4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="11"/>
@@ -5707,43 +5711,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="N1" s="21"/>
     </row>

</xml_diff>